<commit_message>
Setting hake mean length at age 1 to zero
This got rid of compilation errors - trying to fake that the minimum age is 0, since that's not an option in CEATTLE.
</commit_message>
<xml_diff>
--- a/data/hake_singlesp_220310.xlsx
+++ b/data/hake_singlesp_220310.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81D0264D-E4AB-7744-9C33-D6A0D0B24713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68365CD-9B87-AA4C-809D-FC35BD05E5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -4375,7 +4375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AI121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
@@ -14271,8 +14271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14330,19 +14330,19 @@
         <v>308</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>485</v>
+        <v>309</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>485</v>
+        <v>310</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>485</v>
+        <v>311</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>485</v>
+        <v>312</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>485</v>
+        <v>313</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>485</v>
@@ -14380,48 +14380,63 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>23.751773049645401</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>33.104729729729698</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>38.720547945205503</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>42.325513196480898</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>43.435643564356397</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>45.890829694323102</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>50.746987951807199</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>51.690140845070403</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>53.8108108108108</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>55.943396226415103</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>55.461538461538503</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>54.476190476190503</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>54.52</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>54.7826086956522</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
+        <v>56</v>
+      </c>
+      <c r="S2">
+        <v>56</v>
+      </c>
+      <c r="T2">
+        <v>56</v>
+      </c>
+      <c r="U2">
+        <v>56</v>
+      </c>
+      <c r="V2">
         <v>56</v>
       </c>
     </row>

</xml_diff>